<commit_message>
code tidy up and new examples.
</commit_message>
<xml_diff>
--- a/playoffs-example-large.xlsx
+++ b/playoffs-example-large.xlsx
@@ -4066,192 +4066,192 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>28</v>
       </c>
     </row>
-    <row r="5">
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
     <row r="6">
-      <c r="E6" s="24" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="E7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
       <c r="I7" s="20"/>
     </row>
     <row r="8">
-      <c r="I8" s="21">
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>60</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>29</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>29</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>1</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>1</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>76</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>30</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>2</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>2</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>61</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>31</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>3</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -4276,192 +4276,192 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>32</v>
       </c>
     </row>
-    <row r="5">
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
     <row r="6">
-      <c r="E6" s="24" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="E7" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
       <c r="I7" s="20"/>
     </row>
     <row r="8">
-      <c r="I8" s="21">
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>62</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>33</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>33</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>4</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>4</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>77</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>34</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>5</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>5</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>63</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>35</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>6</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -4486,192 +4486,192 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>36</v>
       </c>
     </row>
-    <row r="5">
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
     <row r="6">
-      <c r="E6" s="24" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="E7" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
       <c r="I7" s="20"/>
     </row>
     <row r="8">
-      <c r="I8" s="21">
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>64</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>37</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>37</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>7</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>7</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>78</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>38</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>8</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>8</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>65</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>39</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>9</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -4696,201 +4696,201 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>40</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" s="24" t="s">
+    <row r="6">
+      <c r="C6" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6">
-      <c r="D6" s="22"/>
-      <c r="E6" s="21">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="22"/>
+      <c r="E7" s="21">
         <v>10</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
-      <c r="C7" s="24" t="s">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="20"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8">
-      <c r="I8" s="21">
+      <c r="D8" s="23"/>
+      <c r="E8" s="20"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>66</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>41</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>41</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>11</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>11</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>79</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>42</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>12</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>12</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>67</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>43</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>13</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -4915,192 +4915,192 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>44</v>
       </c>
     </row>
-    <row r="5">
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
     <row r="6">
-      <c r="E6" s="24" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="E7" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
       <c r="I7" s="20"/>
     </row>
     <row r="8">
-      <c r="I8" s="21">
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>68</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>45</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>45</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>14</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>14</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>80</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>46</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>15</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>15</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>69</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>47</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>16</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -5125,201 +5125,201 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>48</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" s="24" t="s">
+    <row r="6">
+      <c r="C6" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6">
-      <c r="D6" s="22"/>
-      <c r="E6" s="21">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="22"/>
+      <c r="E7" s="21">
         <v>17</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
-      <c r="C7" s="24" t="s">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="20"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8">
-      <c r="I8" s="21">
+      <c r="D8" s="23"/>
+      <c r="E8" s="20"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>70</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>49</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>49</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>18</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>18</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>81</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>50</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>19</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>19</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>71</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>51</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>20</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -5344,192 +5344,192 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>52</v>
       </c>
     </row>
-    <row r="5">
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
     <row r="6">
-      <c r="E6" s="24" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="E7" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
       <c r="I7" s="20"/>
     </row>
     <row r="8">
-      <c r="I8" s="21">
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>72</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>53</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>53</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>21</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>21</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>82</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>54</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>22</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>22</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>73</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>55</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>23</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>
@@ -5554,201 +5554,201 @@
     <col customWidth="true" max="2" min="2" width="10"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="E2" s="24" t="s">
+    <row r="3">
+      <c r="E3" s="24" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3">
-      <c r="F3" s="22"/>
-      <c r="G3" s="20"/>
-    </row>
     <row r="4">
-      <c r="G4" s="21">
+      <c r="F4" s="22"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="21">
         <v>56</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" s="24" t="s">
+    <row r="6">
+      <c r="C6" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6">
-      <c r="D6" s="22"/>
-      <c r="E6" s="21">
+      <c r="G6" s="20"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7">
+      <c r="D7" s="22"/>
+      <c r="E7" s="21">
         <v>24</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7">
-      <c r="C7" s="24" t="s">
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="20"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8">
-      <c r="I8" s="21">
+      <c r="D8" s="23"/>
+      <c r="E8" s="20"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9">
+      <c r="I9" s="21">
         <v>74</v>
       </c>
     </row>
-    <row r="9">
-      <c r="I9" s="20"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="20"/>
-    </row>
     <row r="10">
-      <c r="E10" s="24" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
       <c r="I11" s="20"/>
       <c r="K11" s="20"/>
     </row>
     <row r="12">
-      <c r="G12" s="21">
-        <v>57</v>
-      </c>
-      <c r="H12" s="23"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="20"/>
       <c r="I12" s="20"/>
       <c r="K12" s="20"/>
     </row>
     <row r="13">
-      <c r="C13" s="24" t="s">
+      <c r="G13" s="21">
+        <v>57</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14">
-      <c r="D14" s="22"/>
-      <c r="E14" s="21">
-        <v>25</v>
-      </c>
-      <c r="F14" s="23"/>
       <c r="G14" s="20"/>
       <c r="K14" s="20"/>
     </row>
     <row r="15">
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="21">
+        <v>25</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="20"/>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16">
-      <c r="K16" s="21">
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17">
+      <c r="K17" s="21">
         <v>83</v>
       </c>
     </row>
-    <row r="17">
-      <c r="K17" s="20"/>
-    </row>
     <row r="18">
-      <c r="E18" s="24" t="s">
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19">
-      <c r="F19" s="22"/>
-      <c r="G19" s="20"/>
       <c r="K19" s="20"/>
     </row>
     <row r="20">
-      <c r="G20" s="21">
+      <c r="F20" s="22"/>
+      <c r="G20" s="20"/>
+      <c r="K20" s="20"/>
+    </row>
+    <row r="21">
+      <c r="G21" s="21">
         <v>58</v>
       </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="24" t="s">
+      <c r="K21" s="20"/>
+    </row>
+    <row r="22">
+      <c r="C22" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="22"/>
-      <c r="E22" s="21">
-        <v>26</v>
-      </c>
-      <c r="F22" s="23"/>
       <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="20"/>
       <c r="K22" s="20"/>
     </row>
     <row r="23">
-      <c r="C23" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21">
+        <v>26</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24">
-      <c r="I24" s="21">
+      <c r="C24" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="I25" s="21">
         <v>75</v>
       </c>
-      <c r="J24" s="23"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25">
-      <c r="I25" s="20"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26">
-      <c r="E26" s="24" t="s">
+      <c r="I26" s="20"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27">
-      <c r="F27" s="22"/>
-      <c r="G27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28">
-      <c r="G28" s="21">
+      <c r="F28" s="22"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29">
+      <c r="G29" s="21">
         <v>59</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29">
-      <c r="C29" s="24" t="s">
+      <c r="H29" s="23"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="C30" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30">
-      <c r="D30" s="22"/>
-      <c r="E30" s="21">
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="22"/>
+      <c r="E31" s="21">
         <v>27</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31">
-      <c r="C31" s="24" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32">
+      <c r="C32" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="20"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="true" verticalCentered="true"/>

</xml_diff>

<commit_message>
Refactor Excel data handling and improve error management
- Introduced `handleExcelDataError` function to centralize error handling for Excel operations in `excel_data.go`.
- Updated `AddPoolDataToSheet` and `AddPlayerDataToSheet` functions to use the new error handling function.
- Enhanced `CreateTreeBracket`, `writeTreeValue`, and `AddPoolsToTree` functions to handle errors when setting cell styles and formulas.
- Added tests for resource management in the new `resources` package, including file access tests.
- Created a `TournamentService` to encapsulate tournament-related operations and manage Excel client lifecycle.
- Implemented helper functions for creating test data in `helpers.go` to streamline testing.
- Updated `main.go` to utilize the new `resources` package for better resource management.
- Adjusted documentation paths in `mkdocs.yaml` to reflect new structure.
- Updated various Excel files for consistency and testing purposes.
</commit_message>
<xml_diff>
--- a/playoffs-example-large.xlsx
+++ b/playoffs-example-large.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="316">
   <si>
     <t>Elimination Round 1</t>
   </si>
@@ -988,31 +988,13 @@
     <t>Elimination Round 5</t>
   </si>
   <si>
-    <t>Match 84</t>
-  </si>
-  <si>
-    <t>Match 85</t>
-  </si>
-  <si>
-    <t>Match 86</t>
-  </si>
-  <si>
-    <t>Match 87</t>
+    <t>Match 0</t>
   </si>
   <si>
     <t>Elimination Round 6</t>
   </si>
   <si>
-    <t>Match 88</t>
-  </si>
-  <si>
-    <t>Match 89</t>
-  </si>
-  <si>
     <t>Elimination Round 7</t>
-  </si>
-  <si>
-    <t>Match 90</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1219,39 +1201,38 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -1266,7 +1247,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -1334,289 +1314,289 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9756,7 +9736,7 @@
       <c r="F367" s="27"/>
       <c r="G367" s="27"/>
       <c r="I367" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J367" s="27"/>
       <c r="K367" s="27"/>
@@ -9834,7 +9814,7 @@
     <row r="374"/>
     <row r="375">
       <c r="A375" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B375" s="27"/>
       <c r="C375" s="27"/>
@@ -9843,7 +9823,7 @@
       <c r="F375" s="27"/>
       <c r="G375" s="27"/>
       <c r="I375" s="27" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J375" s="27"/>
       <c r="K375" s="27"/>
@@ -9926,7 +9906,7 @@
     <row r="387"/>
     <row r="388">
       <c r="A388" s="27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B388" s="27"/>
       <c r="C388" s="27"/>
@@ -9946,7 +9926,7 @@
     <row r="389"/>
     <row r="390">
       <c r="A390" s="27" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B390" s="27"/>
       <c r="C390" s="27"/>
@@ -9955,7 +9935,7 @@
       <c r="F390" s="27"/>
       <c r="G390" s="27"/>
       <c r="I390" s="27" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="J390" s="27"/>
       <c r="K390" s="27"/>
@@ -9986,7 +9966,7 @@
     </row>
     <row r="392">
       <c r="A392" s="29" t="str">
-        <f>CONCATENATE("M 84 ",'Elimination Matches'!G371)</f>
+        <f>CONCATENATE("M 0 ",'Elimination Matches'!O379)</f>
       </c>
       <c r="B392" s="29"/>
       <c r="C392" s="29"/>
@@ -9994,10 +9974,10 @@
       <c r="E392" s="29"/>
       <c r="F392" s="29"/>
       <c r="G392" s="29" t="str">
-        <f>CONCATENATE("M 85 ",'Elimination Matches'!O371)</f>
+        <f>CONCATENATE("M 0 ",'Elimination Matches'!O379)</f>
       </c>
       <c r="I392" s="29" t="str">
-        <f>CONCATENATE("M 86 ",'Elimination Matches'!G379)</f>
+        <f>CONCATENATE("M 0 ",'Elimination Matches'!G394)</f>
       </c>
       <c r="J392" s="29"/>
       <c r="K392" s="29"/>
@@ -10005,7 +9985,7 @@
       <c r="M392" s="29"/>
       <c r="N392" s="29"/>
       <c r="O392" s="29" t="str">
-        <f>CONCATENATE("M 87 ",'Elimination Matches'!O379)</f>
+        <f>CONCATENATE("M 0 ",'Elimination Matches'!G394)</f>
       </c>
     </row>
     <row r="393"/>
@@ -10038,7 +10018,7 @@
     <row r="402"/>
     <row r="403">
       <c r="A403" s="27" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B403" s="27"/>
       <c r="C403" s="27"/>
@@ -10058,7 +10038,7 @@
     <row r="404"/>
     <row r="405">
       <c r="A405" s="27" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B405" s="27"/>
       <c r="C405" s="27"/>
@@ -10080,7 +10060,7 @@
     </row>
     <row r="407">
       <c r="A407" s="29" t="str">
-        <f>CONCATENATE("M 88 ",'Elimination Matches'!G394)</f>
+        <f>CONCATENATE("M 0 ",'Elimination Matches'!O394)</f>
       </c>
       <c r="B407" s="29"/>
       <c r="C407" s="29"/>
@@ -10088,7 +10068,7 @@
       <c r="E407" s="29"/>
       <c r="F407" s="29"/>
       <c r="G407" s="29" t="str">
-        <f>CONCATENATE("M 89 ",'Elimination Matches'!O394)</f>
+        <f>CONCATENATE("M 0 ",'Elimination Matches'!O394)</f>
       </c>
     </row>
     <row r="408"/>
@@ -10231,7 +10211,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="str">
-        <f>data!DB$2</f>
+        <f>data!D2</f>
       </c>
     </row>
     <row r="2" ht="115" customHeight="true">
@@ -10243,7 +10223,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="str">
-        <f>data!DB$3</f>
+        <f>data!D3</f>
       </c>
     </row>
     <row r="4" ht="115" customHeight="true">
@@ -10255,7 +10235,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="26" t="str">
-        <f>data!DB$4</f>
+        <f>data!D4</f>
       </c>
     </row>
     <row r="6" ht="115" customHeight="true">
@@ -10267,7 +10247,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="26" t="str">
-        <f>data!DB$5</f>
+        <f>data!D5</f>
       </c>
     </row>
     <row r="8" ht="115" customHeight="true">
@@ -10279,7 +10259,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="26" t="str">
-        <f>data!DB$6</f>
+        <f>data!D6</f>
       </c>
     </row>
     <row r="10" ht="115" customHeight="true">
@@ -10291,7 +10271,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="26" t="str">
-        <f>data!DB$7</f>
+        <f>data!D7</f>
       </c>
     </row>
     <row r="12" ht="115" customHeight="true">
@@ -10303,7 +10283,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="26" t="str">
-        <f>data!DB$8</f>
+        <f>data!D8</f>
       </c>
     </row>
     <row r="14" ht="115" customHeight="true">
@@ -10315,7 +10295,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="26" t="str">
-        <f>data!DB$9</f>
+        <f>data!D9</f>
       </c>
     </row>
     <row r="16" ht="115" customHeight="true">
@@ -10327,7 +10307,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="26" t="str">
-        <f>data!DB$10</f>
+        <f>data!D10</f>
       </c>
     </row>
     <row r="18" ht="115" customHeight="true">
@@ -10339,7 +10319,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="26" t="str">
-        <f>data!DB$11</f>
+        <f>data!D11</f>
       </c>
     </row>
     <row r="20" ht="115" customHeight="true">
@@ -10351,7 +10331,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="26" t="str">
-        <f>data!DB$12</f>
+        <f>data!D12</f>
       </c>
     </row>
     <row r="22" ht="115" customHeight="true">
@@ -10363,7 +10343,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="26" t="str">
-        <f>data!DB$13</f>
+        <f>data!D13</f>
       </c>
     </row>
     <row r="24" ht="115" customHeight="true">
@@ -10375,7 +10355,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="26" t="str">
-        <f>data!DB$14</f>
+        <f>data!D14</f>
       </c>
     </row>
     <row r="26" ht="115" customHeight="true">
@@ -10387,7 +10367,7 @@
         <v>13</v>
       </c>
       <c r="B27" s="26" t="str">
-        <f>data!DB$15</f>
+        <f>data!D15</f>
       </c>
     </row>
     <row r="28" ht="115" customHeight="true">
@@ -10399,7 +10379,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="26" t="str">
-        <f>data!DB$16</f>
+        <f>data!D16</f>
       </c>
     </row>
     <row r="30" ht="115" customHeight="true">
@@ -10411,7 +10391,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="26" t="str">
-        <f>data!DB$17</f>
+        <f>data!D17</f>
       </c>
     </row>
     <row r="32" ht="115" customHeight="true">
@@ -10423,7 +10403,7 @@
         <v>16</v>
       </c>
       <c r="B33" s="26" t="str">
-        <f>data!DB$18</f>
+        <f>data!D18</f>
       </c>
     </row>
     <row r="34" ht="115" customHeight="true">
@@ -10435,7 +10415,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="26" t="str">
-        <f>data!DB$19</f>
+        <f>data!D19</f>
       </c>
     </row>
     <row r="36" ht="115" customHeight="true">
@@ -10447,7 +10427,7 @@
         <v>18</v>
       </c>
       <c r="B37" s="26" t="str">
-        <f>data!DB$20</f>
+        <f>data!D20</f>
       </c>
     </row>
     <row r="38" ht="115" customHeight="true">
@@ -10459,7 +10439,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="26" t="str">
-        <f>data!DB$21</f>
+        <f>data!D21</f>
       </c>
     </row>
     <row r="40" ht="115" customHeight="true">
@@ -10471,7 +10451,7 @@
         <v>20</v>
       </c>
       <c r="B41" s="26" t="str">
-        <f>data!DB$22</f>
+        <f>data!D22</f>
       </c>
     </row>
     <row r="42" ht="115" customHeight="true">
@@ -10483,7 +10463,7 @@
         <v>21</v>
       </c>
       <c r="B43" s="26" t="str">
-        <f>data!DB$23</f>
+        <f>data!D23</f>
       </c>
     </row>
     <row r="44" ht="115" customHeight="true">
@@ -10495,7 +10475,7 @@
         <v>22</v>
       </c>
       <c r="B45" s="26" t="str">
-        <f>data!DB$24</f>
+        <f>data!D24</f>
       </c>
     </row>
     <row r="46" ht="115" customHeight="true">
@@ -10507,7 +10487,7 @@
         <v>23</v>
       </c>
       <c r="B47" s="26" t="str">
-        <f>data!DB$25</f>
+        <f>data!D25</f>
       </c>
     </row>
     <row r="48" ht="115" customHeight="true">
@@ -10519,7 +10499,7 @@
         <v>24</v>
       </c>
       <c r="B49" s="26" t="str">
-        <f>data!DB$26</f>
+        <f>data!D26</f>
       </c>
     </row>
     <row r="50" ht="115" customHeight="true">
@@ -10531,7 +10511,7 @@
         <v>25</v>
       </c>
       <c r="B51" s="26" t="str">
-        <f>data!DB$27</f>
+        <f>data!D27</f>
       </c>
     </row>
     <row r="52" ht="115" customHeight="true">
@@ -10543,7 +10523,7 @@
         <v>26</v>
       </c>
       <c r="B53" s="26" t="str">
-        <f>data!DB$28</f>
+        <f>data!D28</f>
       </c>
     </row>
     <row r="54" ht="115" customHeight="true">
@@ -10555,7 +10535,7 @@
         <v>27</v>
       </c>
       <c r="B55" s="26" t="str">
-        <f>data!DB$29</f>
+        <f>data!D29</f>
       </c>
     </row>
     <row r="56" ht="115" customHeight="true">
@@ -10567,7 +10547,7 @@
         <v>28</v>
       </c>
       <c r="B57" s="26" t="str">
-        <f>data!DB$30</f>
+        <f>data!D30</f>
       </c>
     </row>
     <row r="58" ht="115" customHeight="true">
@@ -10579,7 +10559,7 @@
         <v>29</v>
       </c>
       <c r="B59" s="26" t="str">
-        <f>data!DB$31</f>
+        <f>data!D31</f>
       </c>
     </row>
     <row r="60" ht="115" customHeight="true">
@@ -10591,7 +10571,7 @@
         <v>30</v>
       </c>
       <c r="B61" s="26" t="str">
-        <f>data!DB$32</f>
+        <f>data!D32</f>
       </c>
     </row>
     <row r="62" ht="115" customHeight="true">
@@ -10603,7 +10583,7 @@
         <v>31</v>
       </c>
       <c r="B63" s="26" t="str">
-        <f>data!DB$33</f>
+        <f>data!D33</f>
       </c>
     </row>
     <row r="64" ht="115" customHeight="true">
@@ -10615,7 +10595,7 @@
         <v>32</v>
       </c>
       <c r="B65" s="26" t="str">
-        <f>data!DB$34</f>
+        <f>data!D34</f>
       </c>
     </row>
     <row r="66" ht="115" customHeight="true">
@@ -10627,7 +10607,7 @@
         <v>33</v>
       </c>
       <c r="B67" s="26" t="str">
-        <f>data!DB$35</f>
+        <f>data!D35</f>
       </c>
     </row>
     <row r="68" ht="115" customHeight="true">
@@ -10639,7 +10619,7 @@
         <v>34</v>
       </c>
       <c r="B69" s="26" t="str">
-        <f>data!DB$36</f>
+        <f>data!D36</f>
       </c>
     </row>
     <row r="70" ht="115" customHeight="true">
@@ -10651,7 +10631,7 @@
         <v>35</v>
       </c>
       <c r="B71" s="26" t="str">
-        <f>data!DB$37</f>
+        <f>data!D37</f>
       </c>
     </row>
     <row r="72" ht="115" customHeight="true">
@@ -10663,7 +10643,7 @@
         <v>36</v>
       </c>
       <c r="B73" s="26" t="str">
-        <f>data!DB$38</f>
+        <f>data!D38</f>
       </c>
     </row>
     <row r="74" ht="115" customHeight="true">
@@ -10675,7 +10655,7 @@
         <v>37</v>
       </c>
       <c r="B75" s="26" t="str">
-        <f>data!DB$39</f>
+        <f>data!D39</f>
       </c>
     </row>
     <row r="76" ht="115" customHeight="true">
@@ -10687,7 +10667,7 @@
         <v>38</v>
       </c>
       <c r="B77" s="26" t="str">
-        <f>data!DB$40</f>
+        <f>data!D40</f>
       </c>
     </row>
     <row r="78" ht="115" customHeight="true">
@@ -10699,7 +10679,7 @@
         <v>39</v>
       </c>
       <c r="B79" s="26" t="str">
-        <f>data!DB$41</f>
+        <f>data!D41</f>
       </c>
     </row>
     <row r="80" ht="115" customHeight="true">
@@ -10711,7 +10691,7 @@
         <v>40</v>
       </c>
       <c r="B81" s="26" t="str">
-        <f>data!DB$42</f>
+        <f>data!D42</f>
       </c>
     </row>
     <row r="82" ht="115" customHeight="true">
@@ -10723,7 +10703,7 @@
         <v>41</v>
       </c>
       <c r="B83" s="26" t="str">
-        <f>data!DB$43</f>
+        <f>data!D43</f>
       </c>
     </row>
     <row r="84" ht="115" customHeight="true">
@@ -10735,7 +10715,7 @@
         <v>42</v>
       </c>
       <c r="B85" s="26" t="str">
-        <f>data!DB$44</f>
+        <f>data!D44</f>
       </c>
     </row>
     <row r="86" ht="115" customHeight="true">
@@ -10747,7 +10727,7 @@
         <v>43</v>
       </c>
       <c r="B87" s="26" t="str">
-        <f>data!DB$45</f>
+        <f>data!D45</f>
       </c>
     </row>
     <row r="88" ht="115" customHeight="true">
@@ -10759,7 +10739,7 @@
         <v>44</v>
       </c>
       <c r="B89" s="26" t="str">
-        <f>data!DB$46</f>
+        <f>data!D46</f>
       </c>
     </row>
     <row r="90" ht="115" customHeight="true">
@@ -10771,7 +10751,7 @@
         <v>45</v>
       </c>
       <c r="B91" s="26" t="str">
-        <f>data!DB$47</f>
+        <f>data!D47</f>
       </c>
     </row>
     <row r="92" ht="115" customHeight="true">
@@ -10783,7 +10763,7 @@
         <v>46</v>
       </c>
       <c r="B93" s="26" t="str">
-        <f>data!DB$48</f>
+        <f>data!D48</f>
       </c>
     </row>
     <row r="94" ht="115" customHeight="true">
@@ -10795,7 +10775,7 @@
         <v>47</v>
       </c>
       <c r="B95" s="26" t="str">
-        <f>data!DB$49</f>
+        <f>data!D49</f>
       </c>
     </row>
     <row r="96" ht="115" customHeight="true">
@@ -10807,7 +10787,7 @@
         <v>48</v>
       </c>
       <c r="B97" s="26" t="str">
-        <f>data!DB$50</f>
+        <f>data!D50</f>
       </c>
     </row>
     <row r="98" ht="115" customHeight="true">
@@ -10819,7 +10799,7 @@
         <v>49</v>
       </c>
       <c r="B99" s="26" t="str">
-        <f>data!DB$51</f>
+        <f>data!D51</f>
       </c>
     </row>
     <row r="100" ht="115" customHeight="true">
@@ -10831,7 +10811,7 @@
         <v>50</v>
       </c>
       <c r="B101" s="26" t="str">
-        <f>data!DB$52</f>
+        <f>data!D52</f>
       </c>
     </row>
     <row r="102" ht="115" customHeight="true">
@@ -10843,7 +10823,7 @@
         <v>51</v>
       </c>
       <c r="B103" s="26" t="str">
-        <f>data!DB$53</f>
+        <f>data!D53</f>
       </c>
     </row>
     <row r="104" ht="115" customHeight="true">
@@ -10855,7 +10835,7 @@
         <v>52</v>
       </c>
       <c r="B105" s="26" t="str">
-        <f>data!DB$54</f>
+        <f>data!D54</f>
       </c>
     </row>
     <row r="106" ht="115" customHeight="true">
@@ -10867,7 +10847,7 @@
         <v>53</v>
       </c>
       <c r="B107" s="26" t="str">
-        <f>data!DB$55</f>
+        <f>data!D55</f>
       </c>
     </row>
     <row r="108" ht="115" customHeight="true">
@@ -10879,7 +10859,7 @@
         <v>54</v>
       </c>
       <c r="B109" s="26" t="str">
-        <f>data!DB$56</f>
+        <f>data!D56</f>
       </c>
     </row>
     <row r="110" ht="115" customHeight="true">
@@ -10891,7 +10871,7 @@
         <v>55</v>
       </c>
       <c r="B111" s="26" t="str">
-        <f>data!DB$57</f>
+        <f>data!D57</f>
       </c>
     </row>
     <row r="112" ht="115" customHeight="true">
@@ -10903,7 +10883,7 @@
         <v>56</v>
       </c>
       <c r="B113" s="26" t="str">
-        <f>data!DB$58</f>
+        <f>data!D58</f>
       </c>
     </row>
     <row r="114" ht="115" customHeight="true">
@@ -10915,7 +10895,7 @@
         <v>57</v>
       </c>
       <c r="B115" s="26" t="str">
-        <f>data!DB$59</f>
+        <f>data!D59</f>
       </c>
     </row>
     <row r="116" ht="115" customHeight="true">
@@ -10927,7 +10907,7 @@
         <v>58</v>
       </c>
       <c r="B117" s="26" t="str">
-        <f>data!DB$60</f>
+        <f>data!D60</f>
       </c>
     </row>
     <row r="118" ht="115" customHeight="true">
@@ -10939,7 +10919,7 @@
         <v>59</v>
       </c>
       <c r="B119" s="26" t="str">
-        <f>data!DB$61</f>
+        <f>data!D61</f>
       </c>
     </row>
     <row r="120" ht="115" customHeight="true">
@@ -10951,7 +10931,7 @@
         <v>60</v>
       </c>
       <c r="B121" s="26" t="str">
-        <f>data!DB$62</f>
+        <f>data!D62</f>
       </c>
     </row>
     <row r="122" ht="115" customHeight="true">
@@ -10963,7 +10943,7 @@
         <v>61</v>
       </c>
       <c r="B123" s="26" t="str">
-        <f>data!DB$63</f>
+        <f>data!D63</f>
       </c>
     </row>
     <row r="124" ht="115" customHeight="true">
@@ -10975,7 +10955,7 @@
         <v>62</v>
       </c>
       <c r="B125" s="26" t="str">
-        <f>data!DB$64</f>
+        <f>data!D64</f>
       </c>
     </row>
     <row r="126" ht="115" customHeight="true">
@@ -10987,7 +10967,7 @@
         <v>63</v>
       </c>
       <c r="B127" s="26" t="str">
-        <f>data!DB$65</f>
+        <f>data!D65</f>
       </c>
     </row>
     <row r="128" ht="115" customHeight="true">
@@ -10999,7 +10979,7 @@
         <v>64</v>
       </c>
       <c r="B129" s="26" t="str">
-        <f>data!DB$66</f>
+        <f>data!D66</f>
       </c>
     </row>
     <row r="130" ht="115" customHeight="true">
@@ -11011,7 +10991,7 @@
         <v>65</v>
       </c>
       <c r="B131" s="26" t="str">
-        <f>data!DB$67</f>
+        <f>data!D67</f>
       </c>
     </row>
     <row r="132" ht="115" customHeight="true">
@@ -11023,7 +11003,7 @@
         <v>66</v>
       </c>
       <c r="B133" s="26" t="str">
-        <f>data!DB$68</f>
+        <f>data!D68</f>
       </c>
     </row>
     <row r="134" ht="115" customHeight="true">
@@ -11035,7 +11015,7 @@
         <v>67</v>
       </c>
       <c r="B135" s="26" t="str">
-        <f>data!DB$69</f>
+        <f>data!D69</f>
       </c>
     </row>
     <row r="136" ht="115" customHeight="true">
@@ -11047,7 +11027,7 @@
         <v>68</v>
       </c>
       <c r="B137" s="26" t="str">
-        <f>data!DB$70</f>
+        <f>data!D70</f>
       </c>
     </row>
     <row r="138" ht="115" customHeight="true">
@@ -11059,7 +11039,7 @@
         <v>69</v>
       </c>
       <c r="B139" s="26" t="str">
-        <f>data!DB$71</f>
+        <f>data!D71</f>
       </c>
     </row>
     <row r="140" ht="115" customHeight="true">
@@ -11071,7 +11051,7 @@
         <v>70</v>
       </c>
       <c r="B141" s="26" t="str">
-        <f>data!DB$72</f>
+        <f>data!D72</f>
       </c>
     </row>
     <row r="142" ht="115" customHeight="true">
@@ -11083,7 +11063,7 @@
         <v>71</v>
       </c>
       <c r="B143" s="26" t="str">
-        <f>data!DB$73</f>
+        <f>data!D73</f>
       </c>
     </row>
     <row r="144" ht="115" customHeight="true">
@@ -11095,7 +11075,7 @@
         <v>72</v>
       </c>
       <c r="B145" s="26" t="str">
-        <f>data!DB$74</f>
+        <f>data!D74</f>
       </c>
     </row>
     <row r="146" ht="115" customHeight="true">
@@ -11107,7 +11087,7 @@
         <v>73</v>
       </c>
       <c r="B147" s="26" t="str">
-        <f>data!DB$75</f>
+        <f>data!D75</f>
       </c>
     </row>
     <row r="148" ht="115" customHeight="true">
@@ -11119,7 +11099,7 @@
         <v>74</v>
       </c>
       <c r="B149" s="26" t="str">
-        <f>data!DB$76</f>
+        <f>data!D76</f>
       </c>
     </row>
     <row r="150" ht="115" customHeight="true">
@@ -11131,7 +11111,7 @@
         <v>75</v>
       </c>
       <c r="B151" s="26" t="str">
-        <f>data!DB$77</f>
+        <f>data!D77</f>
       </c>
     </row>
     <row r="152" ht="115" customHeight="true">
@@ -11143,7 +11123,7 @@
         <v>76</v>
       </c>
       <c r="B153" s="26" t="str">
-        <f>data!DB$78</f>
+        <f>data!D78</f>
       </c>
     </row>
     <row r="154" ht="115" customHeight="true">
@@ -11155,7 +11135,7 @@
         <v>77</v>
       </c>
       <c r="B155" s="26" t="str">
-        <f>data!DB$79</f>
+        <f>data!D79</f>
       </c>
     </row>
     <row r="156" ht="115" customHeight="true">
@@ -11167,7 +11147,7 @@
         <v>78</v>
       </c>
       <c r="B157" s="26" t="str">
-        <f>data!DB$80</f>
+        <f>data!D80</f>
       </c>
     </row>
     <row r="158" ht="115" customHeight="true">
@@ -11179,7 +11159,7 @@
         <v>79</v>
       </c>
       <c r="B159" s="26" t="str">
-        <f>data!DB$81</f>
+        <f>data!D81</f>
       </c>
     </row>
     <row r="160" ht="115" customHeight="true">
@@ -11191,7 +11171,7 @@
         <v>80</v>
       </c>
       <c r="B161" s="26" t="str">
-        <f>data!DB$82</f>
+        <f>data!D82</f>
       </c>
     </row>
     <row r="162" ht="115" customHeight="true">
@@ -11203,7 +11183,7 @@
         <v>81</v>
       </c>
       <c r="B163" s="26" t="str">
-        <f>data!DB$83</f>
+        <f>data!D83</f>
       </c>
     </row>
     <row r="164" ht="115" customHeight="true">
@@ -11215,7 +11195,7 @@
         <v>82</v>
       </c>
       <c r="B165" s="26" t="str">
-        <f>data!DB$84</f>
+        <f>data!D84</f>
       </c>
     </row>
     <row r="166" ht="115" customHeight="true">
@@ -11227,7 +11207,7 @@
         <v>83</v>
       </c>
       <c r="B167" s="26" t="str">
-        <f>data!DB$85</f>
+        <f>data!D85</f>
       </c>
     </row>
     <row r="168" ht="115" customHeight="true">
@@ -11239,7 +11219,7 @@
         <v>84</v>
       </c>
       <c r="B169" s="26" t="str">
-        <f>data!DB$86</f>
+        <f>data!D86</f>
       </c>
     </row>
     <row r="170" ht="115" customHeight="true">
@@ -11251,7 +11231,7 @@
         <v>85</v>
       </c>
       <c r="B171" s="26" t="str">
-        <f>data!DB$87</f>
+        <f>data!D87</f>
       </c>
     </row>
     <row r="172" ht="115" customHeight="true">
@@ -11263,7 +11243,7 @@
         <v>86</v>
       </c>
       <c r="B173" s="26" t="str">
-        <f>data!DB$88</f>
+        <f>data!D88</f>
       </c>
     </row>
     <row r="174" ht="115" customHeight="true">
@@ -11275,7 +11255,7 @@
         <v>87</v>
       </c>
       <c r="B175" s="26" t="str">
-        <f>data!DB$89</f>
+        <f>data!D89</f>
       </c>
     </row>
     <row r="176" ht="115" customHeight="true">
@@ -11287,7 +11267,7 @@
         <v>88</v>
       </c>
       <c r="B177" s="26" t="str">
-        <f>data!DB$90</f>
+        <f>data!D90</f>
       </c>
     </row>
     <row r="178" ht="115" customHeight="true">
@@ -11299,7 +11279,7 @@
         <v>89</v>
       </c>
       <c r="B179" s="26" t="str">
-        <f>data!DB$91</f>
+        <f>data!D91</f>
       </c>
     </row>
     <row r="180" ht="115" customHeight="true">
@@ -11311,7 +11291,7 @@
         <v>90</v>
       </c>
       <c r="B181" s="26" t="str">
-        <f>data!DB$92</f>
+        <f>data!D92</f>
       </c>
     </row>
     <row r="182" ht="115" customHeight="true">

</xml_diff>

<commit_message>
feat: Generate a new Excel sheet with large, printable player tags and refine existing sheet layouts and player numbering.
</commit_message>
<xml_diff>
--- a/playoffs-example-large.xlsx
+++ b/playoffs-example-large.xlsx
@@ -1006,116 +1006,111 @@
   </numFmts>
   <fonts count="16">
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <u/>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="16"/>
+      <u/>
     </font>
     <font>
-      <b val="1"/>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <u/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <b val="1"/>
       <i val="1"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <sz val="72"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="72"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <sz val="28"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="28"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <family val="2"/>
       <b val="1"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="28"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="110"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <family val="2"/>
       <b val="1"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">

</xml_diff>